<commit_message>
Applied some cosmetic changes
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -43,7 +43,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -60,6 +60,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="00F2AA84"/>
         <bgColor rgb="00F2AA84"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00538DD5"/>
+        <bgColor rgb="00538DD5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCC0DA"/>
+        <bgColor rgb="00CCC0DA"/>
       </patternFill>
     </fill>
   </fills>
@@ -81,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -95,6 +107,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -457,6 +475,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor rgb="00F2AA84"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -468,10 +487,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -616,6 +635,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor rgb="00538DD5"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -627,10 +647,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -877,6 +897,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor rgb="00CCC0DA"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -888,15 +909,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -1027,7 +1048,7 @@
         <v>0.1166666666666671</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>-1.44</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="6">
@@ -1093,7 +1114,7 @@
         <v>0.5666666666666664</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>-5.36</v>
+        <v>5.36</v>
       </c>
     </row>
     <row r="8">
@@ -1126,7 +1147,7 @@
         <v>1.983333333333333</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>-39.8</v>
+        <v>39.8</v>
       </c>
     </row>
     <row r="9">
@@ -1159,7 +1180,7 @@
         <v>3.433333333333334</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>-36.4</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="10">
@@ -1225,7 +1246,7 @@
         <v>4.716666666666667</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>-44.01</v>
+        <v>44.01</v>
       </c>
     </row>
     <row r="12">
@@ -1324,7 +1345,7 @@
         <v>1.566666666666666</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>-16.38</v>
+        <v>16.38</v>
       </c>
     </row>
   </sheetData>
@@ -1341,7 +1362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1349,16 +1370,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="18" customWidth="1" min="9" max="9"/>
-    <col width="18" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -1373,62 +1394,56 @@
       <c r="B2" s="4" t="n"/>
       <c r="C2" s="4" t="n"/>
       <c r="D2" s="4" t="n"/>
-      <c r="E2" s="4" t="n"/>
-      <c r="F2" s="4" t="n"/>
-      <c r="G2" s="4" t="n"/>
-      <c r="H2" s="4" t="n"/>
-      <c r="I2" s="4" t="n"/>
-      <c r="J2" s="4" t="n"/>
+      <c r="E2" s="7" t="n"/>
+      <c r="F2" s="8" t="n"/>
+      <c r="G2" s="8" t="n"/>
+      <c r="H2" s="8" t="n"/>
+      <c r="I2" s="8" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>uid</t>
+          <t>UID</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>servicesPerformed</t>
+          <t>Services Performed</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>attendanceDate</t>
+          <t>Service Date</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>totalSystemHours</t>
+          <t>Invoice Hours</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>totalHoursWorked</t>
+          <t>System Hours</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>variance_hours</t>
+          <t>Variance (Hours)</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>abs_variance_hours</t>
+          <t>Variance (Percentage)</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
-          <t>variance_pct</t>
+          <t>Mismatch Hours</t>
         </is>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>hours_mismatch</t>
-        </is>
-      </c>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t>policy_error</t>
+          <t>Policy Conflict</t>
         </is>
       </c>
     </row>
@@ -1451,18 +1466,15 @@
         <v>8.116666666666667</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>-0.1166666666666671</v>
+        <v>0.1166666666666671</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>0.1166666666666671</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>-1.44</v>
+        <v>1.44</v>
+      </c>
+      <c r="H4" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="I4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1485,18 +1497,15 @@
         <v>10.56666666666667</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>-0.5666666666666664</v>
+        <v>0.5666666666666664</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>0.5666666666666664</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>-5.36</v>
+        <v>5.36</v>
+      </c>
+      <c r="H5" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="I5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1519,18 +1528,15 @@
         <v>4.983333333333333</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>-1.983333333333333</v>
+        <v>1.983333333333333</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>1.983333333333333</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>-39.8</v>
+        <v>39.8</v>
+      </c>
+      <c r="H6" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="I6" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1553,18 +1559,15 @@
         <v>9.433333333333334</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>-3.433333333333334</v>
+        <v>3.433333333333334</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>3.433333333333334</v>
-      </c>
-      <c r="H7" s="5" t="n">
-        <v>-36.4</v>
+        <v>36.4</v>
+      </c>
+      <c r="H7" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="I7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1587,18 +1590,15 @@
         <v>10.71666666666667</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>-4.716666666666667</v>
+        <v>4.716666666666667</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>4.716666666666667</v>
-      </c>
-      <c r="H8" s="5" t="n">
-        <v>-44.01</v>
+        <v>44.01</v>
+      </c>
+      <c r="H8" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="I8" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1621,24 +1621,21 @@
         <v>9.566666666666666</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>-1.566666666666666</v>
+        <v>1.566666666666666</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>1.566666666666666</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <v>-16.38</v>
+        <v>16.38</v>
+      </c>
+      <c r="H9" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="I9" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
changed worksheet name 'Merged' to 'Calculation'
</commit_message>
<xml_diff>
--- a/output/result.xlsx
+++ b/output/result.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Time &amp; Attendance Summary" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SES-Invoice" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Merged" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Calculation" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Comparison" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
@@ -923,7 +923,7 @@
     <row r="1" ht="25" customHeight="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Merged Data</t>
+          <t>Calculated Data</t>
         </is>
       </c>
     </row>

</xml_diff>